<commit_message>
CPI adjusted - compare dollars
</commit_message>
<xml_diff>
--- a/02_script_outputs/01_data/production/median_hh_income_by_race_eth_COMPARE.xlsx
+++ b/02_script_outputs/01_data/production/median_hh_income_by_race_eth_COMPARE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmapil-my.sharepoint.com/personal/sconnelly_cmap_illinois_gov1/Documents/Documents/Local_Projects/ONTO2050-indicators/02_script_outputs/01_data/production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{114F9B8F-1329-43AA-A443-4FF7CD099CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7F0EAAA-73CA-41D7-A5D0-FDE2EC0113E6}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{114F9B8F-1329-43AA-A443-4FF7CD099CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F420BD4E-1471-417A-9E6E-4BB9F4EA2A4B}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="2970" windowWidth="21600" windowHeight="11325" xr2:uid="{7564EE3B-36A5-42AC-91D4-3CD9599A8B49}"/>
+    <workbookView xWindow="3300" yWindow="2520" windowWidth="24225" windowHeight="11880" xr2:uid="{7564EE3B-36A5-42AC-91D4-3CD9599A8B49}"/>
   </bookViews>
   <sheets>
     <sheet name="median_hh_income_by_race_eth_CO" sheetId="1" r:id="rId1"/>
@@ -729,10 +729,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1053,7 +1049,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I10" sqref="I10:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,25 +1318,25 @@
       <c r="G11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11">
         <v>2012</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11">
         <v>61949</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11">
         <v>78844</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11">
         <v>35172</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11">
         <v>47965</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11">
         <v>74105</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" t="s">
         <v>7</v>
       </c>
       <c r="R11" s="7">
@@ -1791,25 +1787,25 @@
       <c r="G18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18">
         <v>2019</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18">
         <v>70765</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18">
         <v>92358</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18">
         <v>39181</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18">
         <v>57007</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18">
         <v>84582</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="O18" t="s">
         <v>7</v>
       </c>
       <c r="R18" s="10">

</xml_diff>